<commit_message>
update CPS data and update html file
</commit_message>
<xml_diff>
--- a/data/CPS/csv_tablename_lookup.xlsx
+++ b/data/CPS/csv_tablename_lookup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunnyshao/Dropbox/CSI State of CE Report share/Data/CPS data/2017_export/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCDD3AB3-07B4-2342-9517-2C71D337A718}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8885245D-99BA-5747-9786-605132B38EEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23800" yWindow="0" windowWidth="17160" windowHeight="23040" xr2:uid="{5716D9BF-6475-B44C-A370-ADE82C6BC670}"/>
+    <workbookView xWindow="29320" yWindow="460" windowWidth="17160" windowHeight="21060" xr2:uid="{5716D9BF-6475-B44C-A370-ADE82C6BC670}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -566,7 +566,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>